<commit_message>
data kepala keluarga filter
</commit_message>
<xml_diff>
--- a/public/files/template/inventory/data_kepala_keluarga.xlsx
+++ b/public/files/template/inventory/data_kepala_keluarga.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">REKAPITULASI PENDATAAN KETOK PINTU </t>
   </si>
@@ -48,30 +48,15 @@
     <t>Provinsi</t>
   </si>
   <si>
-    <t>:</t>
-  </si>
-  <si>
-    <t>[b.kd_prov]</t>
-  </si>
-  <si>
     <t>Kab./Kota</t>
   </si>
   <si>
-    <t>[b.kd_kab]</t>
-  </si>
-  <si>
     <t>Bidang</t>
   </si>
   <si>
-    <t>BIDANG KESEHATAN</t>
-  </si>
-  <si>
     <t>Tanggal Export</t>
   </si>
   <si>
-    <t>[b.tanggal_export]</t>
-  </si>
-  <si>
     <t>RW [b.rw] RT [b.rt]</t>
   </si>
   <si>
@@ -97,6 +82,18 @@
   </si>
   <si>
     <t>PUSKESMAS [b.nama_puskesmas]</t>
+  </si>
+  <si>
+    <t>: [b.kd_prov]</t>
+  </si>
+  <si>
+    <t>: [b.kd_kab]</t>
+  </si>
+  <si>
+    <t>: BIDANG KESEHATAN</t>
+  </si>
+  <si>
+    <t>: [b.tanggal_export]</t>
   </si>
 </sst>
 </file>
@@ -170,38 +167,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -508,7 +513,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +542,7 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="1"/>
@@ -548,7 +553,7 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="10" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="1"/>
@@ -557,124 +562,118 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="C4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="C5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="B6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="12"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>1</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2">
+        <v>3</v>
+      </c>
+      <c r="D10" s="4">
+        <v>4</v>
+      </c>
+      <c r="E10" s="2">
+        <v>5</v>
+      </c>
+      <c r="F10" s="2">
+        <v>6</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="D11" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>1</v>
-      </c>
-      <c r="B10" s="3">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3">
-        <v>3</v>
-      </c>
-      <c r="D10" s="5">
-        <v>4</v>
-      </c>
-      <c r="E10" s="3">
-        <v>5</v>
-      </c>
-      <c r="F10" s="3">
-        <v>6</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="E11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="G11" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chart + db mst pilihan keluarga
</commit_message>
<xml_diff>
--- a/public/files/template/inventory/data_kepala_keluarga.xlsx
+++ b/public/files/template/inventory/data_kepala_keluarga.xlsx
@@ -57,9 +57,6 @@
     <t>Tanggal Export</t>
   </si>
   <si>
-    <t>RW [b.rw] RT [b.rt]</t>
-  </si>
-  <si>
     <t>[a.no;block=tbs:row]</t>
   </si>
   <si>
@@ -94,6 +91,9 @@
   </si>
   <si>
     <t>: [b.tanggal_export]</t>
+  </si>
+  <si>
+    <t>RW [b.rw]</t>
   </si>
 </sst>
 </file>
@@ -513,7 +513,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,7 +542,7 @@
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="1"/>
@@ -553,7 +553,7 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="10" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="1"/>
@@ -566,7 +566,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -578,7 +578,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -590,7 +590,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -601,7 +601,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -655,25 +655,25 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="F11" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="G11" s="8" t="s">
         <v>19</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>